<commit_message>
change sense resistor and Mosfet
</commit_message>
<xml_diff>
--- a/board/Project Outputs for Einsy_Rambo_0.5c/BOM/Einsy Rambo_projectVersion.xlsx
+++ b/board/Project Outputs for Einsy_Rambo_0.5c/BOM/Einsy Rambo_projectVersion.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="939" uniqueCount="554">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="939" uniqueCount="553">
   <si>
     <t>Designator</t>
   </si>
@@ -865,28 +865,31 @@
     <t>Q1, Q5</t>
   </si>
   <si>
-    <t>1727-4635-2-ND</t>
+    <t>1727-1052-2-ND</t>
   </si>
   <si>
     <t>Nexperia</t>
   </si>
   <si>
-    <t>PSMN7R0-60YS,115</t>
-  </si>
-  <si>
-    <t>PSMN7R0-60</t>
+    <t>PSMN1R8-40YLC,115</t>
+  </si>
+  <si>
+    <t>PSMN1R8-40YLC</t>
   </si>
   <si>
     <t>SOT669</t>
   </si>
   <si>
-    <t>Mosfet N-channel 60V 356A 117W 9.3mOhms</t>
-  </si>
-  <si>
-    <t>N-Channel 60V 89A (Tc) 117W (Tc) Surface Mount LFPAK56, Power-SO8</t>
-  </si>
-  <si>
-    <t>60V 89A N-CHAN</t>
+    <t>MOSFET N-CH 40V 100A LFPAK</t>
+  </si>
+  <si>
+    <t>N-Channel 40V 100A (Tc) 272W (Tc) Surface Mount LFPAK56, Power-SO8</t>
+  </si>
+  <si>
+    <t>N-FET</t>
+  </si>
+  <si>
+    <t>40V 100A 1.8mOhm</t>
   </si>
   <si>
     <t>Q2</t>
@@ -1039,25 +1042,19 @@
     <t>R7, R10, R15, R17, R18, R22, R25, R26</t>
   </si>
   <si>
-    <t>P17624TR-ND</t>
+    <t>RUT3216FR220CS</t>
   </si>
   <si>
     <t>Panasonic</t>
   </si>
   <si>
-    <t>ERJ-8BQFR22V</t>
-  </si>
-  <si>
     <t>0.22R</t>
   </si>
   <si>
     <t>R1206</t>
   </si>
   <si>
-    <t>RES SMD 0.22 OHM 1% 1/2W 1206</t>
-  </si>
-  <si>
-    <t>0.22 Ohm ±1% 0.5W, 1/2W Chip Resistor 1206 (3216 Metric) Automotive AEC-Q200, Current Sense Thick Film</t>
+    <t>RES SMD 0.22 OHM 1% 1/3W 1206</t>
   </si>
   <si>
     <t>0.22R 1% 1206</t>
@@ -3612,7 +3609,7 @@
         <v>282</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>16</v>
+        <v>232</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>283</v>
@@ -3624,7 +3621,7 @@
         <v>285</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>286</v>
+        <v>21</v>
       </c>
       <c r="G34" s="3">
         <v>2</v>
@@ -3633,7 +3630,7 @@
         <v>21</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="J34" s="2" t="s">
         <v>287</v>
@@ -3645,33 +3642,33 @@
         <v>289</v>
       </c>
       <c r="M34" s="2" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
       <c r="N34" s="2" t="s">
-        <v>121</v>
+        <v>192</v>
       </c>
       <c r="O34" s="2" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="35" spans="1:15">
       <c r="A35" s="2" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="G35" s="3">
         <v>1</v>
@@ -3680,45 +3677,45 @@
         <v>21</v>
       </c>
       <c r="I35" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="J35" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="K35" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="L35" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="M35" s="2" t="s">
         <v>296</v>
-      </c>
-      <c r="J35" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="K35" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="L35" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="M35" s="2" t="s">
-        <v>295</v>
       </c>
       <c r="N35" s="2" t="s">
         <v>121</v>
       </c>
       <c r="O35" s="2" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="36" spans="1:15">
       <c r="A36" s="2" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="G36" s="3">
         <v>6</v>
@@ -3727,45 +3724,45 @@
         <v>21</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="J36" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="K36" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="L36" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="M36" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="K36" s="2" t="s">
-        <v>306</v>
-      </c>
-      <c r="L36" s="2" t="s">
-        <v>307</v>
-      </c>
-      <c r="M36" s="2" t="s">
-        <v>304</v>
-      </c>
       <c r="N36" s="2" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="O36" s="2" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
     </row>
     <row r="37" spans="1:15">
       <c r="A37" s="2" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="G37" s="3">
         <v>1</v>
@@ -3774,45 +3771,45 @@
         <v>21</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="K37" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="L37" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="M37" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="L37" s="2" t="s">
-        <v>316</v>
-      </c>
-      <c r="M37" s="2" t="s">
-        <v>314</v>
-      </c>
       <c r="N37" s="2" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="O37" s="2" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="38" spans="1:15">
       <c r="A38" s="2" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="G38" s="3">
         <v>4</v>
@@ -3821,45 +3818,45 @@
         <v>21</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="K38" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="L38" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="M38" s="2" t="s">
         <v>322</v>
       </c>
-      <c r="L38" s="2" t="s">
-        <v>323</v>
-      </c>
-      <c r="M38" s="2" t="s">
-        <v>321</v>
-      </c>
       <c r="N38" s="2" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="O38" s="2" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="39" spans="1:15">
       <c r="A39" s="2" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="G39" s="3">
         <v>5</v>
@@ -3868,45 +3865,45 @@
         <v>21</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="K39" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="L39" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="M39" s="2" t="s">
         <v>329</v>
       </c>
-      <c r="L39" s="2" t="s">
-        <v>330</v>
-      </c>
-      <c r="M39" s="2" t="s">
-        <v>328</v>
-      </c>
       <c r="N39" s="2" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="O39" s="2" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
     </row>
     <row r="40" spans="1:15">
       <c r="A40" s="2" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="G40" s="3">
         <v>11</v>
@@ -3915,42 +3912,42 @@
         <v>21</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="K40" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="L40" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="M40" s="2" t="s">
         <v>337</v>
       </c>
-      <c r="L40" s="2" t="s">
-        <v>338</v>
-      </c>
-      <c r="M40" s="2" t="s">
-        <v>336</v>
-      </c>
       <c r="N40" s="2" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="O40" s="2" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
     </row>
     <row r="41" spans="1:15">
       <c r="A41" s="2" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="D41" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="E41" s="2" t="s">
         <v>342</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>343</v>
       </c>
       <c r="F41" s="2" t="s">
         <v>344</v>
@@ -3971,36 +3968,36 @@
         <v>346</v>
       </c>
       <c r="L41" s="2" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="M41" s="2" t="s">
         <v>344</v>
       </c>
       <c r="N41" s="2" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="O41" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="42" spans="1:15">
       <c r="A42" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C42" s="2" t="s">
         <v>349</v>
       </c>
-      <c r="B42" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C42" s="2" t="s">
+      <c r="D42" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="E42" s="2" t="s">
         <v>350</v>
       </c>
-      <c r="D42" s="2" t="s">
-        <v>302</v>
-      </c>
-      <c r="E42" s="2" t="s">
+      <c r="F42" s="2" t="s">
         <v>351</v>
-      </c>
-      <c r="F42" s="2" t="s">
-        <v>352</v>
       </c>
       <c r="G42" s="3">
         <v>7</v>
@@ -4009,45 +4006,45 @@
         <v>21</v>
       </c>
       <c r="I42" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="J42" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="K42" s="2" t="s">
         <v>353</v>
       </c>
-      <c r="J42" s="2" t="s">
-        <v>305</v>
-      </c>
-      <c r="K42" s="2" t="s">
+      <c r="L42" s="2" t="s">
         <v>354</v>
       </c>
-      <c r="L42" s="2" t="s">
+      <c r="M42" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="N42" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="O42" s="2" t="s">
         <v>355</v>
-      </c>
-      <c r="M42" s="2" t="s">
-        <v>353</v>
-      </c>
-      <c r="N42" s="2" t="s">
-        <v>308</v>
-      </c>
-      <c r="O42" s="2" t="s">
-        <v>356</v>
       </c>
     </row>
     <row r="43" spans="1:15">
       <c r="A43" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C43" s="2" t="s">
         <v>357</v>
       </c>
-      <c r="B43" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C43" s="2" t="s">
+      <c r="D43" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="E43" s="2" t="s">
         <v>358</v>
       </c>
-      <c r="D43" s="2" t="s">
-        <v>302</v>
-      </c>
-      <c r="E43" s="2" t="s">
+      <c r="F43" s="2" t="s">
         <v>359</v>
-      </c>
-      <c r="F43" s="2" t="s">
-        <v>360</v>
       </c>
       <c r="G43" s="3">
         <v>15</v>
@@ -4056,45 +4053,45 @@
         <v>21</v>
       </c>
       <c r="I43" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="J43" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="K43" s="2" t="s">
         <v>361</v>
       </c>
-      <c r="J43" s="2" t="s">
-        <v>305</v>
-      </c>
-      <c r="K43" s="2" t="s">
+      <c r="L43" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="L43" s="2" t="s">
+      <c r="M43" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="N43" s="2" t="s">
         <v>363</v>
       </c>
-      <c r="M43" s="2" t="s">
-        <v>361</v>
-      </c>
-      <c r="N43" s="2" t="s">
+      <c r="O43" s="2" t="s">
         <v>364</v>
-      </c>
-      <c r="O43" s="2" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="44" spans="1:15">
       <c r="A44" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C44" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="B44" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C44" s="2" t="s">
+      <c r="D44" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="E44" s="2" t="s">
         <v>367</v>
       </c>
-      <c r="D44" s="2" t="s">
-        <v>302</v>
-      </c>
-      <c r="E44" s="2" t="s">
+      <c r="F44" s="2" t="s">
         <v>368</v>
-      </c>
-      <c r="F44" s="2" t="s">
-        <v>369</v>
       </c>
       <c r="G44" s="3">
         <v>1</v>
@@ -4103,45 +4100,45 @@
         <v>21</v>
       </c>
       <c r="I44" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="J44" s="2" t="s">
         <v>369</v>
       </c>
-      <c r="J44" s="2" t="s">
+      <c r="K44" s="2" t="s">
         <v>370</v>
       </c>
-      <c r="K44" s="2" t="s">
+      <c r="L44" s="2" t="s">
         <v>371</v>
       </c>
-      <c r="L44" s="2" t="s">
+      <c r="M44" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="N44" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="O44" s="2" t="s">
         <v>372</v>
-      </c>
-      <c r="M44" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="N44" s="2" t="s">
-        <v>364</v>
-      </c>
-      <c r="O44" s="2" t="s">
-        <v>373</v>
       </c>
     </row>
     <row r="45" spans="1:15">
       <c r="A45" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C45" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="B45" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C45" s="2" t="s">
+      <c r="D45" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="E45" s="2" t="s">
         <v>375</v>
       </c>
-      <c r="D45" s="2" t="s">
-        <v>302</v>
-      </c>
-      <c r="E45" s="2" t="s">
+      <c r="F45" s="2" t="s">
         <v>376</v>
-      </c>
-      <c r="F45" s="2" t="s">
-        <v>377</v>
       </c>
       <c r="G45" s="3">
         <v>8</v>
@@ -4150,45 +4147,45 @@
         <v>21</v>
       </c>
       <c r="I45" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="J45" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="K45" s="2" t="s">
         <v>378</v>
       </c>
-      <c r="J45" s="2" t="s">
-        <v>305</v>
-      </c>
-      <c r="K45" s="2" t="s">
+      <c r="L45" s="2" t="s">
         <v>379</v>
       </c>
-      <c r="L45" s="2" t="s">
-        <v>380</v>
-      </c>
       <c r="M45" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="N45" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="O45" s="2" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="46" spans="1:15">
       <c r="A46" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C46" s="2" t="s">
         <v>381</v>
       </c>
-      <c r="B46" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C46" s="2" t="s">
+      <c r="D46" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="E46" s="2" t="s">
         <v>382</v>
       </c>
-      <c r="D46" s="2" t="s">
-        <v>302</v>
-      </c>
-      <c r="E46" s="2" t="s">
+      <c r="F46" s="2" t="s">
         <v>383</v>
-      </c>
-      <c r="F46" s="2" t="s">
-        <v>384</v>
       </c>
       <c r="G46" s="3">
         <v>7</v>
@@ -4197,45 +4194,45 @@
         <v>21</v>
       </c>
       <c r="I46" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="J46" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="K46" s="2" t="s">
         <v>385</v>
       </c>
-      <c r="J46" s="2" t="s">
-        <v>305</v>
-      </c>
-      <c r="K46" s="2" t="s">
+      <c r="L46" s="2" t="s">
         <v>386</v>
       </c>
-      <c r="L46" s="2" t="s">
+      <c r="M46" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="N46" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="O46" s="2" t="s">
         <v>387</v>
-      </c>
-      <c r="M46" s="2" t="s">
-        <v>385</v>
-      </c>
-      <c r="N46" s="2" t="s">
-        <v>308</v>
-      </c>
-      <c r="O46" s="2" t="s">
-        <v>388</v>
       </c>
     </row>
     <row r="47" spans="1:15">
       <c r="A47" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C47" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="B47" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C47" s="2" t="s">
+      <c r="D47" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="E47" s="2" t="s">
         <v>390</v>
       </c>
-      <c r="D47" s="2" t="s">
-        <v>302</v>
-      </c>
-      <c r="E47" s="2" t="s">
+      <c r="F47" s="2" t="s">
         <v>391</v>
-      </c>
-      <c r="F47" s="2" t="s">
-        <v>392</v>
       </c>
       <c r="G47" s="3">
         <v>4</v>
@@ -4244,45 +4241,45 @@
         <v>21</v>
       </c>
       <c r="I47" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="J47" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="K47" s="2" t="s">
         <v>392</v>
       </c>
-      <c r="J47" s="2" t="s">
-        <v>305</v>
-      </c>
-      <c r="K47" s="2" t="s">
+      <c r="L47" s="2" t="s">
         <v>393</v>
       </c>
-      <c r="L47" s="2" t="s">
+      <c r="M47" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="N47" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="O47" s="2" t="s">
         <v>394</v>
-      </c>
-      <c r="M47" s="2" t="s">
-        <v>392</v>
-      </c>
-      <c r="N47" s="2" t="s">
-        <v>308</v>
-      </c>
-      <c r="O47" s="2" t="s">
-        <v>395</v>
       </c>
     </row>
     <row r="48" spans="1:15">
       <c r="A48" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C48" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="E48" s="2" t="s">
         <v>358</v>
       </c>
-      <c r="D48" s="2" t="s">
-        <v>302</v>
-      </c>
-      <c r="E48" s="2" t="s">
+      <c r="F48" s="2" t="s">
         <v>359</v>
-      </c>
-      <c r="F48" s="2" t="s">
-        <v>360</v>
       </c>
       <c r="G48" s="3">
         <v>2</v>
@@ -4291,45 +4288,45 @@
         <v>7</v>
       </c>
       <c r="I48" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="J48" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="K48" s="2" t="s">
         <v>361</v>
       </c>
-      <c r="J48" s="2" t="s">
-        <v>305</v>
-      </c>
-      <c r="K48" s="2" t="s">
+      <c r="L48" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="L48" s="2" t="s">
+      <c r="M48" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="N48" s="2" t="s">
         <v>363</v>
       </c>
-      <c r="M48" s="2" t="s">
-        <v>361</v>
-      </c>
-      <c r="N48" s="2" t="s">
+      <c r="O48" s="2" t="s">
         <v>364</v>
-      </c>
-      <c r="O48" s="2" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="49" spans="1:15">
       <c r="A49" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C49" s="2" t="s">
         <v>397</v>
       </c>
-      <c r="B49" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C49" s="2" t="s">
+      <c r="D49" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="E49" s="2" t="s">
         <v>398</v>
       </c>
-      <c r="D49" s="2" t="s">
-        <v>342</v>
-      </c>
-      <c r="E49" s="2" t="s">
+      <c r="F49" s="2" t="s">
         <v>399</v>
-      </c>
-      <c r="F49" s="2" t="s">
-        <v>400</v>
       </c>
       <c r="G49" s="3">
         <v>1</v>
@@ -4338,45 +4335,45 @@
         <v>21</v>
       </c>
       <c r="I49" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="J49" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="K49" s="2" t="s">
         <v>400</v>
       </c>
-      <c r="J49" s="2" t="s">
-        <v>305</v>
-      </c>
-      <c r="K49" s="2" t="s">
+      <c r="L49" s="2" t="s">
         <v>401</v>
       </c>
-      <c r="L49" s="2" t="s">
+      <c r="M49" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="N49" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="O49" s="2" t="s">
         <v>402</v>
-      </c>
-      <c r="M49" s="2" t="s">
-        <v>400</v>
-      </c>
-      <c r="N49" s="2" t="s">
-        <v>308</v>
-      </c>
-      <c r="O49" s="2" t="s">
-        <v>403</v>
       </c>
     </row>
     <row r="50" spans="1:15">
       <c r="A50" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C50" s="2" t="s">
         <v>404</v>
       </c>
-      <c r="B50" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C50" s="2" t="s">
+      <c r="D50" s="2" t="s">
         <v>405</v>
       </c>
-      <c r="D50" s="2" t="s">
+      <c r="E50" s="2" t="s">
         <v>406</v>
       </c>
-      <c r="E50" s="2" t="s">
+      <c r="F50" s="2" t="s">
         <v>407</v>
-      </c>
-      <c r="F50" s="2" t="s">
-        <v>408</v>
       </c>
       <c r="G50" s="3">
         <v>2</v>
@@ -4385,45 +4382,45 @@
         <v>21</v>
       </c>
       <c r="I50" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="J50" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="J50" s="2" t="s">
+      <c r="K50" s="2" t="s">
         <v>409</v>
       </c>
-      <c r="K50" s="2" t="s">
+      <c r="L50" s="2" t="s">
         <v>410</v>
       </c>
-      <c r="L50" s="2" t="s">
+      <c r="M50" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="N50" s="2" t="s">
         <v>411</v>
       </c>
-      <c r="M50" s="2" t="s">
-        <v>408</v>
-      </c>
-      <c r="N50" s="2" t="s">
+      <c r="O50" s="2" t="s">
         <v>412</v>
-      </c>
-      <c r="O50" s="2" t="s">
-        <v>413</v>
       </c>
     </row>
     <row r="51" spans="1:15">
       <c r="A51" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C51" s="2" t="s">
         <v>414</v>
       </c>
-      <c r="B51" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C51" s="2" t="s">
+      <c r="D51" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="E51" s="2" t="s">
         <v>415</v>
       </c>
-      <c r="D51" s="2" t="s">
-        <v>406</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>416</v>
-      </c>
       <c r="F51" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="G51" s="3">
         <v>1</v>
@@ -4432,45 +4429,45 @@
         <v>21</v>
       </c>
       <c r="I51" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="J51" s="2" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="K51" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="L51" s="2" t="s">
         <v>417</v>
       </c>
-      <c r="L51" s="2" t="s">
+      <c r="M51" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="N51" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="O51" s="2" t="s">
         <v>418</v>
-      </c>
-      <c r="M51" s="2" t="s">
-        <v>361</v>
-      </c>
-      <c r="N51" s="2" t="s">
-        <v>412</v>
-      </c>
-      <c r="O51" s="2" t="s">
-        <v>419</v>
       </c>
     </row>
     <row r="52" spans="1:15">
       <c r="A52" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C52" s="2" t="s">
         <v>420</v>
       </c>
-      <c r="B52" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C52" s="2" t="s">
+      <c r="D52" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="E52" s="2" t="s">
         <v>421</v>
       </c>
-      <c r="D52" s="2" t="s">
-        <v>406</v>
-      </c>
-      <c r="E52" s="2" t="s">
-        <v>422</v>
-      </c>
       <c r="F52" s="2" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="G52" s="3">
         <v>1</v>
@@ -4479,45 +4476,45 @@
         <v>21</v>
       </c>
       <c r="I52" s="2" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="J52" s="2" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="K52" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="L52" s="2" t="s">
         <v>423</v>
       </c>
-      <c r="L52" s="2" t="s">
+      <c r="M52" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="N52" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="O52" s="2" t="s">
         <v>424</v>
-      </c>
-      <c r="M52" s="2" t="s">
-        <v>385</v>
-      </c>
-      <c r="N52" s="2" t="s">
-        <v>412</v>
-      </c>
-      <c r="O52" s="2" t="s">
-        <v>425</v>
       </c>
     </row>
     <row r="53" spans="1:15">
       <c r="A53" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C53" s="2" t="s">
         <v>426</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>427</v>
       </c>
       <c r="D53" s="2" t="s">
         <v>72</v>
       </c>
       <c r="E53" s="2" t="s">
+        <v>427</v>
+      </c>
+      <c r="F53" s="2" t="s">
         <v>428</v>
-      </c>
-      <c r="F53" s="2" t="s">
-        <v>429</v>
       </c>
       <c r="G53" s="3">
         <v>3</v>
@@ -4526,45 +4523,45 @@
         <v>21</v>
       </c>
       <c r="I53" s="2" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="J53" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="K53" s="2" t="s">
         <v>430</v>
       </c>
-      <c r="K53" s="2" t="s">
+      <c r="L53" s="2" t="s">
         <v>431</v>
       </c>
-      <c r="L53" s="2" t="s">
+      <c r="M53" s="2" t="s">
         <v>432</v>
-      </c>
-      <c r="M53" s="2" t="s">
-        <v>433</v>
       </c>
       <c r="N53" s="2" t="s">
         <v>121</v>
       </c>
       <c r="O53" s="2" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="54" spans="1:15">
       <c r="A54" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C54" s="2" t="s">
         <v>434</v>
       </c>
-      <c r="B54" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C54" s="2" t="s">
+      <c r="D54" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="E54" s="2" t="s">
         <v>435</v>
       </c>
-      <c r="D54" s="2" t="s">
-        <v>302</v>
-      </c>
-      <c r="E54" s="2" t="s">
+      <c r="F54" s="2" t="s">
         <v>436</v>
-      </c>
-      <c r="F54" s="2" t="s">
-        <v>437</v>
       </c>
       <c r="G54" s="3">
         <v>4</v>
@@ -4573,45 +4570,45 @@
         <v>21</v>
       </c>
       <c r="I54" s="2" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="J54" s="2" t="s">
         <v>23</v>
       </c>
       <c r="K54" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="L54" s="2" t="s">
         <v>438</v>
       </c>
-      <c r="L54" s="2" t="s">
-        <v>439</v>
-      </c>
       <c r="M54" s="2" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="N54" s="2" t="s">
         <v>121</v>
       </c>
       <c r="O54" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="55" spans="1:15">
       <c r="A55" s="2" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>232</v>
       </c>
       <c r="C55" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="D55" s="2" t="s">
         <v>442</v>
       </c>
-      <c r="D55" s="2" t="s">
+      <c r="E55" s="2" t="s">
         <v>443</v>
       </c>
-      <c r="E55" s="2" t="s">
+      <c r="F55" s="2" t="s">
         <v>444</v>
-      </c>
-      <c r="F55" s="2" t="s">
-        <v>445</v>
       </c>
       <c r="G55" s="3">
         <v>16</v>
@@ -4623,13 +4620,13 @@
         <v>188</v>
       </c>
       <c r="J55" s="2" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="K55" s="2" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="L55" s="2" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="M55" s="2" t="s">
         <v>191</v>
@@ -4638,27 +4635,27 @@
         <v>192</v>
       </c>
       <c r="O55" s="2" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="56" spans="1:15">
       <c r="A56" s="2" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B56" s="2" t="s">
         <v>232</v>
       </c>
       <c r="C56" s="2" t="s">
+        <v>448</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="E56" s="2" t="s">
         <v>449</v>
       </c>
-      <c r="D56" s="2" t="s">
-        <v>342</v>
-      </c>
-      <c r="E56" s="2" t="s">
+      <c r="F56" s="2" t="s">
         <v>450</v>
-      </c>
-      <c r="F56" s="2" t="s">
-        <v>451</v>
       </c>
       <c r="G56" s="3">
         <v>1</v>
@@ -4667,22 +4664,22 @@
         <v>21</v>
       </c>
       <c r="I56" s="2" t="s">
+        <v>450</v>
+      </c>
+      <c r="J56" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="K56" s="2" t="s">
         <v>451</v>
       </c>
-      <c r="J56" s="2" t="s">
-        <v>305</v>
-      </c>
-      <c r="K56" s="2" t="s">
+      <c r="L56" s="2" t="s">
         <v>452</v>
       </c>
-      <c r="L56" s="2" t="s">
-        <v>453</v>
-      </c>
       <c r="M56" s="2" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="N56" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="O56" s="2" t="s">
         <v>21</v>
@@ -4690,22 +4687,22 @@
     </row>
     <row r="57" spans="1:15">
       <c r="A57" s="2" t="s">
+        <v>453</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C57" s="2" t="s">
         <v>454</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>455</v>
       </c>
       <c r="D57" s="2" t="s">
         <v>196</v>
       </c>
       <c r="E57" s="2" t="s">
+        <v>455</v>
+      </c>
+      <c r="F57" s="2" t="s">
         <v>456</v>
-      </c>
-      <c r="F57" s="2" t="s">
-        <v>457</v>
       </c>
       <c r="G57" s="3">
         <v>1</v>
@@ -4714,45 +4711,45 @@
         <v>21</v>
       </c>
       <c r="I57" s="2" t="s">
+        <v>455</v>
+      </c>
+      <c r="J57" s="2" t="s">
+        <v>457</v>
+      </c>
+      <c r="K57" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="L57" s="2" t="s">
+        <v>459</v>
+      </c>
+      <c r="M57" s="2" t="s">
         <v>456</v>
-      </c>
-      <c r="J57" s="2" t="s">
-        <v>458</v>
-      </c>
-      <c r="K57" s="2" t="s">
-        <v>459</v>
-      </c>
-      <c r="L57" s="2" t="s">
-        <v>460</v>
-      </c>
-      <c r="M57" s="2" t="s">
-        <v>457</v>
       </c>
       <c r="N57" s="2" t="s">
         <v>121</v>
       </c>
       <c r="O57" s="2" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="58" spans="1:15">
       <c r="A58" s="2" t="s">
+        <v>461</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C58" s="2" t="s">
         <v>462</v>
       </c>
-      <c r="B58" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C58" s="2" t="s">
+      <c r="D58" s="2" t="s">
         <v>463</v>
       </c>
-      <c r="D58" s="2" t="s">
+      <c r="E58" s="2" t="s">
         <v>464</v>
       </c>
-      <c r="E58" s="2" t="s">
+      <c r="F58" s="2" t="s">
         <v>465</v>
-      </c>
-      <c r="F58" s="2" t="s">
-        <v>466</v>
       </c>
       <c r="G58" s="3">
         <v>1</v>
@@ -4761,45 +4758,45 @@
         <v>21</v>
       </c>
       <c r="I58" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="J58" s="2" t="s">
         <v>467</v>
       </c>
-      <c r="J58" s="2" t="s">
+      <c r="K58" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="L58" s="2" t="s">
         <v>468</v>
       </c>
-      <c r="K58" s="2" t="s">
-        <v>467</v>
-      </c>
-      <c r="L58" s="2" t="s">
-        <v>469</v>
-      </c>
       <c r="M58" s="2" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="N58" s="2" t="s">
         <v>121</v>
       </c>
       <c r="O58" s="2" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="59" spans="1:15">
       <c r="A59" s="2" t="s">
+        <v>470</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C59" s="2" t="s">
         <v>471</v>
       </c>
-      <c r="B59" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C59" s="2" t="s">
+      <c r="D59" s="2" t="s">
+        <v>463</v>
+      </c>
+      <c r="E59" s="2" t="s">
         <v>472</v>
       </c>
-      <c r="D59" s="2" t="s">
-        <v>464</v>
-      </c>
-      <c r="E59" s="2" t="s">
+      <c r="F59" s="2" t="s">
         <v>473</v>
-      </c>
-      <c r="F59" s="2" t="s">
-        <v>474</v>
       </c>
       <c r="G59" s="3">
         <v>1</v>
@@ -4808,45 +4805,45 @@
         <v>21</v>
       </c>
       <c r="I59" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="J59" s="2" t="s">
         <v>475</v>
       </c>
-      <c r="J59" s="2" t="s">
+      <c r="K59" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="L59" s="2" t="s">
         <v>476</v>
       </c>
-      <c r="K59" s="2" t="s">
-        <v>475</v>
-      </c>
-      <c r="L59" s="2" t="s">
-        <v>477</v>
-      </c>
       <c r="M59" s="2" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="N59" s="2" t="s">
         <v>121</v>
       </c>
       <c r="O59" s="2" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="60" spans="1:15">
       <c r="A60" s="2" t="s">
+        <v>478</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C60" s="2" t="s">
         <v>479</v>
       </c>
-      <c r="B60" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C60" s="2" t="s">
+      <c r="D60" s="2" t="s">
         <v>480</v>
       </c>
-      <c r="D60" s="2" t="s">
+      <c r="E60" s="2" t="s">
         <v>481</v>
       </c>
-      <c r="E60" s="2" t="s">
+      <c r="F60" s="2" t="s">
         <v>482</v>
-      </c>
-      <c r="F60" s="2" t="s">
-        <v>483</v>
       </c>
       <c r="G60" s="3">
         <v>1</v>
@@ -4855,45 +4852,45 @@
         <v>21</v>
       </c>
       <c r="I60" s="2" t="s">
+        <v>482</v>
+      </c>
+      <c r="J60" s="2" t="s">
         <v>483</v>
       </c>
-      <c r="J60" s="2" t="s">
+      <c r="K60" s="2" t="s">
         <v>484</v>
       </c>
-      <c r="K60" s="2" t="s">
+      <c r="L60" s="2" t="s">
         <v>485</v>
       </c>
-      <c r="L60" s="2" t="s">
-        <v>486</v>
-      </c>
       <c r="M60" s="2" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="N60" s="2" t="s">
         <v>121</v>
       </c>
       <c r="O60" s="2" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="61" spans="1:15">
       <c r="A61" s="2" t="s">
+        <v>487</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C61" s="2" t="s">
         <v>488</v>
       </c>
-      <c r="B61" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C61" s="2" t="s">
+      <c r="D61" s="2" t="s">
         <v>489</v>
       </c>
-      <c r="D61" s="2" t="s">
+      <c r="E61" s="2" t="s">
         <v>490</v>
       </c>
-      <c r="E61" s="2" t="s">
+      <c r="F61" s="2" t="s">
         <v>491</v>
-      </c>
-      <c r="F61" s="2" t="s">
-        <v>492</v>
       </c>
       <c r="G61" s="3">
         <v>4</v>
@@ -4902,45 +4899,45 @@
         <v>21</v>
       </c>
       <c r="I61" s="2" t="s">
+        <v>492</v>
+      </c>
+      <c r="J61" s="2" t="s">
         <v>493</v>
       </c>
-      <c r="J61" s="2" t="s">
+      <c r="K61" s="2" t="s">
         <v>494</v>
       </c>
-      <c r="K61" s="2" t="s">
+      <c r="L61" s="2" t="s">
         <v>495</v>
       </c>
-      <c r="L61" s="2" t="s">
-        <v>496</v>
-      </c>
       <c r="M61" s="2" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="N61" s="2" t="s">
         <v>121</v>
       </c>
       <c r="O61" s="2" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="62" spans="1:15">
       <c r="A62" s="2" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>232</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D62" s="2" t="s">
         <v>284</v>
       </c>
       <c r="E62" s="2" t="s">
+        <v>499</v>
+      </c>
+      <c r="F62" s="2" t="s">
         <v>500</v>
-      </c>
-      <c r="F62" s="2" t="s">
-        <v>501</v>
       </c>
       <c r="G62" s="3">
         <v>1</v>
@@ -4949,16 +4946,16 @@
         <v>21</v>
       </c>
       <c r="I62" s="2" t="s">
+        <v>500</v>
+      </c>
+      <c r="J62" s="2" t="s">
         <v>501</v>
       </c>
-      <c r="J62" s="2" t="s">
+      <c r="K62" s="2" t="s">
         <v>502</v>
       </c>
-      <c r="K62" s="2" t="s">
+      <c r="L62" s="2" t="s">
         <v>503</v>
-      </c>
-      <c r="L62" s="2" t="s">
-        <v>504</v>
       </c>
       <c r="M62" s="2" t="s">
         <v>192</v>
@@ -4967,27 +4964,27 @@
         <v>192</v>
       </c>
       <c r="O62" s="2" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="63" spans="1:15">
       <c r="A63" s="2" t="s">
+        <v>505</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C63" s="2" t="s">
         <v>506</v>
       </c>
-      <c r="B63" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C63" s="2" t="s">
+      <c r="D63" s="2" t="s">
         <v>507</v>
       </c>
-      <c r="D63" s="2" t="s">
+      <c r="E63" s="2" t="s">
         <v>508</v>
       </c>
-      <c r="E63" s="2" t="s">
+      <c r="F63" s="2" t="s">
         <v>509</v>
-      </c>
-      <c r="F63" s="2" t="s">
-        <v>510</v>
       </c>
       <c r="G63" s="3">
         <v>1</v>
@@ -4996,45 +4993,45 @@
         <v>21</v>
       </c>
       <c r="I63" s="2" t="s">
+        <v>510</v>
+      </c>
+      <c r="J63" s="2" t="s">
         <v>511</v>
       </c>
-      <c r="J63" s="2" t="s">
+      <c r="K63" s="2" t="s">
         <v>512</v>
       </c>
-      <c r="K63" s="2" t="s">
+      <c r="L63" s="2" t="s">
         <v>513</v>
       </c>
-      <c r="L63" s="2" t="s">
-        <v>514</v>
-      </c>
       <c r="M63" s="2" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="N63" s="2" t="s">
         <v>121</v>
       </c>
       <c r="O63" s="2" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="64" spans="1:15">
       <c r="A64" s="2" t="s">
+        <v>515</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C64" s="2" t="s">
         <v>516</v>
       </c>
-      <c r="B64" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C64" s="2" t="s">
+      <c r="D64" s="2" t="s">
         <v>517</v>
       </c>
-      <c r="D64" s="2" t="s">
+      <c r="E64" s="2" t="s">
         <v>518</v>
       </c>
-      <c r="E64" s="2" t="s">
+      <c r="F64" s="2" t="s">
         <v>519</v>
-      </c>
-      <c r="F64" s="2" t="s">
-        <v>520</v>
       </c>
       <c r="G64" s="3">
         <v>1</v>
@@ -5043,45 +5040,45 @@
         <v>21</v>
       </c>
       <c r="I64" s="2" t="s">
+        <v>519</v>
+      </c>
+      <c r="J64" s="2" t="s">
         <v>520</v>
       </c>
-      <c r="J64" s="2" t="s">
+      <c r="K64" s="2" t="s">
         <v>521</v>
       </c>
-      <c r="K64" s="2" t="s">
+      <c r="L64" s="2" t="s">
         <v>522</v>
       </c>
-      <c r="L64" s="2" t="s">
-        <v>523</v>
-      </c>
       <c r="M64" s="2" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="N64" s="2" t="s">
         <v>121</v>
       </c>
       <c r="O64" s="2" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="65" spans="1:15">
       <c r="A65" s="2" t="s">
+        <v>524</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C65" s="2" t="s">
         <v>525</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C65" s="2" t="s">
-        <v>526</v>
       </c>
       <c r="D65" s="2" t="s">
         <v>206</v>
       </c>
       <c r="E65" s="2" t="s">
+        <v>526</v>
+      </c>
+      <c r="F65" s="2" t="s">
         <v>527</v>
-      </c>
-      <c r="F65" s="2" t="s">
-        <v>528</v>
       </c>
       <c r="G65" s="3">
         <v>1</v>
@@ -5090,45 +5087,45 @@
         <v>21</v>
       </c>
       <c r="I65" s="2" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="J65" s="2" t="s">
+        <v>528</v>
+      </c>
+      <c r="K65" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="K65" s="2" t="s">
+      <c r="L65" s="2" t="s">
         <v>530</v>
       </c>
-      <c r="L65" s="2" t="s">
-        <v>531</v>
-      </c>
       <c r="M65" s="2" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="N65" s="2" t="s">
         <v>121</v>
       </c>
       <c r="O65" s="2" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="66" spans="1:15">
       <c r="A66" s="2" t="s">
+        <v>532</v>
+      </c>
+      <c r="B66" s="2" t="s">
         <v>533</v>
       </c>
-      <c r="B66" s="2" t="s">
+      <c r="C66" s="2" t="s">
         <v>534</v>
       </c>
-      <c r="C66" s="2" t="s">
+      <c r="D66" s="2" t="s">
         <v>535</v>
       </c>
-      <c r="D66" s="2" t="s">
+      <c r="E66" s="2" t="s">
         <v>536</v>
       </c>
-      <c r="E66" s="2" t="s">
+      <c r="F66" s="2" t="s">
         <v>537</v>
-      </c>
-      <c r="F66" s="2" t="s">
-        <v>538</v>
       </c>
       <c r="G66" s="3">
         <v>1</v>
@@ -5137,45 +5134,45 @@
         <v>21</v>
       </c>
       <c r="I66" s="2" t="s">
+        <v>538</v>
+      </c>
+      <c r="J66" s="2" t="s">
         <v>539</v>
       </c>
-      <c r="J66" s="2" t="s">
+      <c r="K66" s="2" t="s">
         <v>540</v>
       </c>
-      <c r="K66" s="2" t="s">
+      <c r="L66" s="2" t="s">
         <v>541</v>
       </c>
-      <c r="L66" s="2" t="s">
-        <v>542</v>
-      </c>
       <c r="M66" s="2" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="N66" s="2" t="s">
         <v>121</v>
       </c>
       <c r="O66" s="2" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="67" spans="1:15">
       <c r="A67" s="2" t="s">
+        <v>543</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C67" s="2" t="s">
         <v>544</v>
       </c>
-      <c r="B67" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C67" s="2" t="s">
+      <c r="D67" s="2" t="s">
         <v>545</v>
       </c>
-      <c r="D67" s="2" t="s">
+      <c r="E67" s="2" t="s">
         <v>546</v>
       </c>
-      <c r="E67" s="2" t="s">
+      <c r="F67" s="2" t="s">
         <v>547</v>
-      </c>
-      <c r="F67" s="2" t="s">
-        <v>548</v>
       </c>
       <c r="G67" s="3">
         <v>2</v>
@@ -5184,29 +5181,29 @@
         <v>21</v>
       </c>
       <c r="I67" s="2" t="s">
+        <v>546</v>
+      </c>
+      <c r="J67" s="2" t="s">
+        <v>548</v>
+      </c>
+      <c r="K67" s="2" t="s">
+        <v>549</v>
+      </c>
+      <c r="L67" s="2" t="s">
+        <v>550</v>
+      </c>
+      <c r="M67" s="2" t="s">
         <v>547</v>
       </c>
-      <c r="J67" s="2" t="s">
-        <v>549</v>
-      </c>
-      <c r="K67" s="2" t="s">
-        <v>550</v>
-      </c>
-      <c r="L67" s="2" t="s">
+      <c r="N67" s="2" t="s">
         <v>551</v>
       </c>
-      <c r="M67" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="N67" s="2" t="s">
+      <c r="O67" s="2" t="s">
         <v>552</v>
-      </c>
-      <c r="O67" s="2" t="s">
-        <v>553</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>